<commit_message>
SanofiNZ Green Cross Failing
</commit_message>
<xml_diff>
--- a/Projects/SANOFINZ/Data/Template.xlsx
+++ b/Projects/SANOFINZ/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -531,7 +531,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="107">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -864,7 +864,7 @@
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -968,21 +968,6 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1134,7 +1119,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1168,13 +1153,6 @@
       <right/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -1263,7 +1241,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="77">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1392,23 +1370,39 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="8" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="18" fillId="9" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1416,34 +1410,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="20" fillId="9" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="9" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1452,7 +1422,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="21" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1460,95 +1430,95 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="26" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="24" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="7" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="8" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="26" fillId="8" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="8" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="8" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1675,19 +1645,19 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1945,18 +1915,18 @@
   </sheetPr>
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.0242914979757"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2849,17 +2819,17 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="26" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="31.8137651821862"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="26" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="27" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2889,168 +2859,172 @@
       <c r="E2" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="33"/>
+      <c r="F2" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="34"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="39"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="39"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="39"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="39"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="34"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="39"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="34"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="39"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="34"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="39"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="34"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="39"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="34"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="39"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="34"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="39"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="34"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="39"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="34"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="34"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="39"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="39"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="34"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="39"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="39"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="39"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="34"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="39"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="34"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="39"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="37"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3069,28 +3043,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="45" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="45" width="51.8461538461539"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="45" width="39.5263157894737"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="45" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="46" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="43" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="52.2753036437247"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="39.8502024291498"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="44" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47"/>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="48" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="46" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3110,30 +3084,35 @@
       <c r="E2" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="32"/>
+      <c r="F2" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="47" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="47" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="47" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="47" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="47" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3156,349 +3135,349 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="51" width="32.9919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="51" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="51" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="52" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="48" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="49" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="48" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="49" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="49" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="48" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="50" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="53"/>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="54" t="s">
+      <c r="A1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="54"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="54" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="61" t="n">
+      <c r="F3" s="59" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="50" t="n">
+      <c r="G3" s="48" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="61" t="n">
+      <c r="F4" s="59" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="50" t="n">
+      <c r="G4" s="48" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="50" t="n">
+      <c r="F5" s="59" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="48" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="50" t="n">
+      <c r="F6" s="59" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="48" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="60" t="s">
+      <c r="E7" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="50" t="n">
+      <c r="F7" s="59" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="48" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="E8" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="50" t="n">
+      <c r="F8" s="59" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="48" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="E9" s="60" t="s">
+      <c r="E9" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="F9" s="61" t="n">
+      <c r="F9" s="59" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="50" t="n">
+      <c r="G9" s="48" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="62"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="66"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="64"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="62"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="66"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="64"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="62"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="66"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="64"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="62"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="66"/>
+      <c r="A13" s="60"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="64"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="62"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="66"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="64"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="62"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="64"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="62"/>
-      <c r="B16" s="63"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="64"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="62"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="66"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="64"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="62"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="66"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="64"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="62"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="66"/>
+      <c r="A19" s="60"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="64"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="62"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="66"/>
+      <c r="A20" s="60"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="64"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="62"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="66"/>
+      <c r="A21" s="60"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="64"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="62"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="66"/>
+      <c r="A22" s="60"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="64"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="62"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="70"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="68"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="62"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="66"/>
+      <c r="A24" s="60"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="64"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="62"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="66"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="64"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F26" s="71"/>
+      <c r="F26" s="69"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="71"/>
+      <c r="F27" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3522,20 +3501,20 @@
   </sheetPr>
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="32.0283400809717"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.0242914979757"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="32.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="1023" min="7" style="14" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="72" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="70" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3550,19 +3529,19 @@
       <c r="G1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="73" t="s">
+      <c r="E2" s="71" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="18" t="s">
@@ -3573,19 +3552,19 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="76" t="n">
+      <c r="C3" s="74" t="n">
         <v>9300655602477</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="73" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="23" t="n">
@@ -3596,19 +3575,19 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="76" t="n">
+      <c r="C4" s="74" t="n">
         <v>93301992</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="75" t="s">
+      <c r="E4" s="73" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="23" t="n">
@@ -3619,19 +3598,19 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="76" t="n">
+      <c r="C5" s="74" t="n">
         <v>9319733003273</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="77" t="s">
+      <c r="E5" s="75" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="23" t="n">
@@ -3642,19 +3621,19 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="74" t="s">
+      <c r="A6" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="76" t="n">
+      <c r="C6" s="74" t="n">
         <v>9310717300005</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="77" t="s">
+      <c r="E6" s="75" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="23" t="n">
@@ -3665,19 +3644,19 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="76" t="n">
+      <c r="C7" s="74" t="n">
         <v>9310717300029</v>
       </c>
-      <c r="D7" s="75" t="s">
+      <c r="D7" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="75" t="s">
+      <c r="E7" s="73" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="23" t="n">
@@ -3688,19 +3667,19 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="76" t="n">
+      <c r="C8" s="74" t="n">
         <v>9416270112120</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="75" t="s">
+      <c r="E8" s="73" t="s">
         <v>48</v>
       </c>
       <c r="F8" s="23" t="n">
@@ -3711,19 +3690,19 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="76" t="n">
+      <c r="C9" s="74" t="n">
         <v>9416270112113</v>
       </c>
-      <c r="D9" s="75" t="s">
+      <c r="D9" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="75" t="s">
+      <c r="E9" s="73" t="s">
         <v>48</v>
       </c>
       <c r="F9" s="23" t="n">
@@ -3734,19 +3713,19 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="74" t="s">
+      <c r="A10" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="76" t="n">
+      <c r="C10" s="74" t="n">
         <v>9316090019220</v>
       </c>
-      <c r="D10" s="75" t="s">
+      <c r="D10" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="75" t="s">
+      <c r="E10" s="73" t="s">
         <v>52</v>
       </c>
       <c r="F10" s="23" t="n">
@@ -3757,19 +3736,19 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="76" t="n">
+      <c r="C11" s="74" t="n">
         <v>9316090019350</v>
       </c>
-      <c r="D11" s="75" t="s">
+      <c r="D11" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="73" t="s">
         <v>54</v>
       </c>
       <c r="F11" s="23" t="n">
@@ -3780,19 +3759,19 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="76" t="n">
+      <c r="C12" s="74" t="n">
         <v>9316090016175</v>
       </c>
-      <c r="D12" s="75" t="s">
+      <c r="D12" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="75" t="s">
+      <c r="E12" s="73" t="s">
         <v>54</v>
       </c>
       <c r="F12" s="23" t="n">
@@ -3803,19 +3782,19 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="76" t="n">
+      <c r="C13" s="74" t="n">
         <v>9316090018759</v>
       </c>
-      <c r="D13" s="75" t="s">
+      <c r="D13" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="77" t="s">
+      <c r="E13" s="75" t="s">
         <v>54</v>
       </c>
       <c r="F13" s="23" t="n">
@@ -3826,19 +3805,19 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="75" t="s">
+      <c r="B14" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="76" t="n">
+      <c r="C14" s="74" t="n">
         <v>9316090019237</v>
       </c>
-      <c r="D14" s="75" t="s">
+      <c r="D14" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="77" t="s">
+      <c r="E14" s="75" t="s">
         <v>52</v>
       </c>
       <c r="F14" s="23" t="n">
@@ -3849,19 +3828,19 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="76" t="n">
+      <c r="C15" s="74" t="n">
         <v>9316090019237</v>
       </c>
-      <c r="D15" s="75" t="s">
+      <c r="D15" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="75" t="s">
+      <c r="E15" s="73" t="s">
         <v>52</v>
       </c>
       <c r="F15" s="23" t="n">
@@ -3872,19 +3851,19 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="74" t="s">
+      <c r="A16" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="76" t="n">
+      <c r="C16" s="74" t="n">
         <v>9316090019190</v>
       </c>
-      <c r="D16" s="75" t="s">
+      <c r="D16" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="75" t="s">
+      <c r="E16" s="73" t="s">
         <v>52</v>
       </c>
       <c r="F16" s="23" t="n">
@@ -3895,19 +3874,19 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="74" t="s">
+      <c r="A17" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="76" t="n">
+      <c r="C17" s="74" t="n">
         <v>9316090021100</v>
       </c>
-      <c r="D17" s="75" t="s">
+      <c r="D17" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="75" t="s">
+      <c r="E17" s="73" t="s">
         <v>62</v>
       </c>
       <c r="F17" s="23" t="n">
@@ -3918,19 +3897,19 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="74" t="s">
+      <c r="A18" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="76" t="n">
+      <c r="C18" s="74" t="n">
         <v>9316090019206</v>
       </c>
-      <c r="D18" s="75" t="s">
+      <c r="D18" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="75" t="s">
+      <c r="E18" s="73" t="s">
         <v>52</v>
       </c>
       <c r="F18" s="23" t="n">
@@ -3941,19 +3920,19 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="76" t="n">
+      <c r="C19" s="74" t="n">
         <v>9319733001903</v>
       </c>
-      <c r="D19" s="75" t="s">
+      <c r="D19" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="75" t="s">
+      <c r="E19" s="73" t="s">
         <v>41</v>
       </c>
       <c r="F19" s="23" t="n">
@@ -3964,19 +3943,19 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="74" t="s">
+      <c r="A20" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="76" t="n">
+      <c r="C20" s="74" t="n">
         <v>9300655003298</v>
       </c>
-      <c r="D20" s="75" t="s">
+      <c r="D20" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="75" t="s">
+      <c r="E20" s="73" t="s">
         <v>41</v>
       </c>
       <c r="F20" s="23" t="n">
@@ -3987,19 +3966,19 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="76" t="n">
+      <c r="C21" s="74" t="n">
         <v>9300655059240</v>
       </c>
-      <c r="D21" s="75" t="s">
+      <c r="D21" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="77" t="s">
+      <c r="E21" s="75" t="s">
         <v>41</v>
       </c>
       <c r="F21" s="23" t="n">
@@ -4010,19 +3989,19 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="74" t="s">
+      <c r="A22" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="75" t="s">
+      <c r="B22" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="76" t="n">
+      <c r="C22" s="74" t="n">
         <v>9300655122548</v>
       </c>
-      <c r="D22" s="75" t="s">
+      <c r="D22" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="75" t="s">
+      <c r="E22" s="73" t="s">
         <v>39</v>
       </c>
       <c r="F22" s="23" t="n">
@@ -4033,19 +4012,19 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="75" t="s">
+      <c r="B23" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="76" t="n">
+      <c r="C23" s="74" t="n">
         <v>9300655056812</v>
       </c>
-      <c r="D23" s="75" t="s">
+      <c r="D23" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="75" t="s">
+      <c r="E23" s="73" t="s">
         <v>39</v>
       </c>
       <c r="F23" s="23" t="n">
@@ -4056,19 +4035,19 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="74" t="s">
+      <c r="A24" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="75" t="s">
+      <c r="B24" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="76" t="n">
+      <c r="C24" s="74" t="n">
         <v>9321547072611</v>
       </c>
-      <c r="D24" s="75" t="s">
+      <c r="D24" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="75" t="s">
+      <c r="E24" s="73" t="s">
         <v>71</v>
       </c>
       <c r="F24" s="23" t="n">
@@ -4079,19 +4058,19 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="74" t="s">
+      <c r="A25" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="75" t="s">
+      <c r="B25" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="76" t="n">
+      <c r="C25" s="74" t="n">
         <v>9321547136023</v>
       </c>
-      <c r="D25" s="75" t="s">
+      <c r="D25" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="75" t="s">
+      <c r="E25" s="73" t="s">
         <v>74</v>
       </c>
       <c r="F25" s="23" t="n">
@@ -4102,19 +4081,19 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="75" t="s">
+      <c r="B26" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="76" t="n">
+      <c r="C26" s="74" t="n">
         <v>9321547146213</v>
       </c>
-      <c r="D26" s="75" t="s">
+      <c r="D26" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="75" t="s">
+      <c r="E26" s="73" t="s">
         <v>74</v>
       </c>
       <c r="F26" s="23" t="n">
@@ -4125,19 +4104,19 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="74" t="s">
+      <c r="A27" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="78" t="s">
+      <c r="B27" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="76" t="n">
+      <c r="C27" s="74" t="n">
         <v>9319733002290</v>
       </c>
-      <c r="D27" s="77" t="s">
+      <c r="D27" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="E27" s="77" t="s">
+      <c r="E27" s="75" t="s">
         <v>74</v>
       </c>
       <c r="F27" s="23" t="n">
@@ -4148,19 +4127,19 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="74" t="s">
+      <c r="A28" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="78" t="s">
+      <c r="B28" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="76" t="n">
+      <c r="C28" s="74" t="n">
         <v>9417133903442</v>
       </c>
-      <c r="D28" s="77" t="s">
+      <c r="D28" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="E28" s="77" t="s">
+      <c r="E28" s="75" t="s">
         <v>74</v>
       </c>
       <c r="F28" s="23" t="n">

</xml_diff>